<commit_message>
Subo reporte de bugs encontrados
</commit_message>
<xml_diff>
--- a/bugs/reporte_bugs.xlsx
+++ b/bugs/reporte_bugs.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29725"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mayra\Desktop\ProyectoFinal-ChazarretaMayra\bugs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C3F66FCD-C560-4E4A-ADC9-22108FEFEF40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -18,9 +24,161 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="49">
+  <si>
+    <t>Reporte de bugs</t>
+  </si>
+  <si>
+    <t>Resultado Esperado</t>
+  </si>
+  <si>
+    <t>Resultado Obtenido</t>
+  </si>
+  <si>
+    <t>Titulo descriptivo</t>
+  </si>
+  <si>
+    <t>Pasos para reproducir</t>
+  </si>
+  <si>
+    <t>Severidad</t>
+  </si>
+  <si>
+    <t>Evidencia</t>
+  </si>
+  <si>
+    <t>1) Abrir app 2)Ir a registro 3) Completar nro de celular repetido 4) Completar fecha de nacimiento 5) Completar nombre y apellido 6) Crear contraseña válida 7) Registrarse</t>
+  </si>
+  <si>
+    <t>Se muestra error por numero de celular ya registrado previamente</t>
+  </si>
+  <si>
+    <t>Se registra con éxito</t>
+  </si>
+  <si>
+    <t>Alta</t>
+  </si>
+  <si>
+    <t>https://trello.com/c/wsRlCaKP</t>
+  </si>
+  <si>
+    <t>Se registran varias cuentas con un mismo numero de celular</t>
+  </si>
+  <si>
+    <t>La contraseña debe incluir numeros pero no lo pide en ciertos casos</t>
+  </si>
+  <si>
+    <t>1)Abrir app 2)Ir a registro 3)Completar campos requeridos 4)Crear contraseña sin números</t>
+  </si>
+  <si>
+    <t>Se muestra error, la contraseña requiere al menos 1 numero</t>
+  </si>
+  <si>
+    <t>https://trello.com/c/TeHrnAtD</t>
+  </si>
+  <si>
+    <t>Luego de 3 login incorrectos no se bloquea la cuenta</t>
+  </si>
+  <si>
+    <t>1)Abrir app. 2)Completar Usuario y Contraseña incorrectas</t>
+  </si>
+  <si>
+    <t>Excediste el limite de intentos. Bloquearemos tu cuenta por seguridad</t>
+  </si>
+  <si>
+    <t>No se bloquea, permite volver a intentarlo o el envio de un email para restaurar contraseña</t>
+  </si>
+  <si>
+    <t>https://trello.com/c/oDvw5XTF</t>
+  </si>
+  <si>
+    <t>1)Abrir app. 2)Completar Usuario y Contraseña correctas</t>
+  </si>
+  <si>
+    <t>Tu cuenta está bloqueada. Tenemos que confirmar tu identidad</t>
+  </si>
+  <si>
+    <t>Inicio normal. Deberia permanecer bloqueado</t>
+  </si>
+  <si>
+    <t>https://trello.com/c/z6PunwCB</t>
+  </si>
+  <si>
+    <t>No toma medidas de seguridad para volver a iniciar luego de un bloqueo</t>
+  </si>
+  <si>
+    <t>1)Abrir app 2)Editar perfil 3)Genero personalizado 4)Guardar</t>
+  </si>
+  <si>
+    <t>Muestra error y pide indicar un genero valido</t>
+  </si>
+  <si>
+    <t>Permite poner cualquier cosa en genero. Ej:gato</t>
+  </si>
+  <si>
+    <t>Permite cargar cualquier cosa. No valida generos</t>
+  </si>
+  <si>
+    <t>Baja</t>
+  </si>
+  <si>
+    <t>https://trello.com/c/z2D5Jk0p</t>
+  </si>
+  <si>
+    <t>1)Abrir app 2)Seleccionar publicacion 3)Editar</t>
+  </si>
+  <si>
+    <t>Se espera poder añadir musica</t>
+  </si>
+  <si>
+    <t>Cada vez que toco para editar, arroja error</t>
+  </si>
+  <si>
+    <t>Quiero agregar musica a una publicacion existente, se tilda y marca error</t>
+  </si>
+  <si>
+    <t>https://trello.com/c/cVpgSHWh</t>
+  </si>
+  <si>
+    <t>Quiero silenciar musica/audio de un post y falla</t>
+  </si>
+  <si>
+    <t>1)Seleccionar publicacion 2)Boton para silenciar musica/audio</t>
+  </si>
+  <si>
+    <t>Permite cancelar el sonido</t>
+  </si>
+  <si>
+    <t>Al presionar el símbolo del parlante, no se silencia la musica.</t>
+  </si>
+  <si>
+    <t>https://trello.com/c/s5VgAfzD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1)Seleccionar comentario </t>
+  </si>
+  <si>
+    <t>El sistema no me permite editar mi comentario</t>
+  </si>
+  <si>
+    <t>Permite cambiar el texto y guardarlo</t>
+  </si>
+  <si>
+    <t>No existe la accion de editar, solo permite eliminarlo</t>
+  </si>
+  <si>
+    <t>https://trello.com/c/Azb9cQsa</t>
+  </si>
+  <si>
+    <t>Crítica</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,16 +186,77 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="0"/>
+      <name val="Abadi"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="7"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCA71ED"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9A57CD"/>
+        <bgColor rgb="FFD5A6BD"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,18 +264,85 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF9A57CD"/>
+      <color rgb="FFCA71ED"/>
+      <color rgb="FFF999B0"/>
+      <color rgb="FFE894DC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -66,6 +352,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -330,13 +620,271 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="A1:G3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="30.85546875" customWidth="1"/>
+    <col min="3" max="3" width="34.28515625" customWidth="1"/>
+    <col min="4" max="4" width="33.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="10"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="10"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="10"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F2"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="F4" r:id="rId1" xr:uid="{4C7D2864-B1BD-4004-8385-6A6CA9D43AC1}"/>
+    <hyperlink ref="F5" r:id="rId2" xr:uid="{AC5FE5DB-3F67-42E3-B487-B270BB417A32}"/>
+    <hyperlink ref="F6" r:id="rId3" xr:uid="{A2C82835-AA3C-4890-8625-4897D35AA15E}"/>
+    <hyperlink ref="F7" r:id="rId4" xr:uid="{554F02DC-FD20-4F28-B126-6F2E734D7A01}"/>
+    <hyperlink ref="F8" r:id="rId5" xr:uid="{EF431B51-385A-4D06-AE78-4E11273F569D}"/>
+    <hyperlink ref="F9" r:id="rId6" xr:uid="{42A7C5C9-E771-4761-968B-51F0F512D935}"/>
+    <hyperlink ref="F10" r:id="rId7" xr:uid="{CFB26D31-3053-44BF-953D-A79DDFC1C607}"/>
+    <hyperlink ref="F11" r:id="rId8" xr:uid="{64D351AB-83A7-406B-AA5A-7200B7945DFB}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>